<commit_message>
just befor sprint2 review
</commit_message>
<xml_diff>
--- a/doc/r2_scaffold.xlsx
+++ b/doc/r2_scaffold.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="211">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="3"/>
@@ -1535,12 +1535,182 @@
     <t>rake db:schema:load</t>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rails generate migration add_invoice_no_to_engineorders </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF990073"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>invoice_no</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:string</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rails generate migration add_day_of_test_to_engineorders </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF990073"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>day_of_test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:string</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>受注クラスに、送り状Noと試運転日を追加</t>
+    <rPh sb="0" eb="2">
+      <t>ジュチュウ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>オク</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ジョウ</t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t>シウンテン</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ビ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rails generate migration add_shipped_date_to_engineorders </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF990073"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>shipped_date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:date</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rails generate migration add_shipped_date_to_repairs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF990073"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>shipped_date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:date</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rails generate migration add_day_of_test_to_engineorders </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF990073"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>day_of_test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:date</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">rails generate migration remove_day_of_test_from_engineorders </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF990073"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>day_of_test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>:string</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1648,6 +1818,12 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1711,7 +1887,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1746,6 +1922,9 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2051,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM100"/>
+  <dimension ref="A1:AM113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4247,7 +4426,7 @@
       <c r="Y95" s="3"/>
       <c r="Z95" s="5"/>
     </row>
-    <row r="97" spans="5:26">
+    <row r="97" spans="2:26">
       <c r="E97" s="3" t="s">
         <v>197</v>
       </c>
@@ -4281,7 +4460,7 @@
       <c r="Y97" s="3"/>
       <c r="Z97" s="5"/>
     </row>
-    <row r="98" spans="5:26">
+    <row r="98" spans="2:26">
       <c r="E98" s="10" t="s">
         <v>198</v>
       </c>
@@ -4325,10 +4504,66 @@
       <c r="Y98" s="3"/>
       <c r="Z98" s="5"/>
     </row>
-    <row r="100" spans="5:26">
+    <row r="100" spans="2:26">
       <c r="E100" s="6" t="str">
         <f>CONCATENATE($A$1,C95," ",E95,F95,G95,H95,I95,J95,K95,L95,M95,N95,O95,P95,Q95,R95,S95,T95,U95,V95,W95,X95,Y95,Z95) &amp; CONCATENATE(E98,F98,G98,H98,I98,J98,K98,L98)</f>
         <v xml:space="preserve">rails generate scaffold Engineorder issueNo:string inquiryDate:date loginUserId:integer branchCode:integer userId:integer placeCode:integer orderer:string machineNo:string timeOfRunning:integer changeComment:text orderDate:date sendingCompanyCode:integer sendingComment:text deliveryDate:date </v>
+      </c>
+    </row>
+    <row r="102" spans="2:26">
+      <c r="C102" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="2:26" ht="15" thickBot="1">
+      <c r="B103" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="104" spans="2:26" ht="15" thickBot="1">
+      <c r="C104" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="105" spans="2:26" ht="15" thickBot="1">
+      <c r="C105" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="106" spans="2:26" ht="15" thickBot="1">
+      <c r="C106" s="17"/>
+    </row>
+    <row r="107" spans="2:26" ht="15" thickBot="1">
+      <c r="B107" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="108" spans="2:26" ht="15" thickBot="1">
+      <c r="C108" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="Y108" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="2:26" ht="15" thickBot="1">
+      <c r="C109" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y109" s="1" t="str">
+        <f>CONCATENATE(W109," ",E109,F109,G109,H109,I109,J109,K109,L109,M109,N109,O109,P109,Q109,R109,,S109,T109,U109,V109,W109,X109)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="111" spans="2:26" ht="15" thickBot="1"/>
+    <row r="112" spans="2:26" ht="15" thickBot="1">
+      <c r="C112" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" ht="15" thickBot="1">
+      <c r="C113" s="17" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug on Engine Arrived when Repair not exist
</commit_message>
<xml_diff>
--- a/doc/r2_scaffold.xlsx
+++ b/doc/r2_scaffold.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@gitwork\merge\r2\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="105" windowWidth="19395" windowHeight="8025"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="r2" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -25,7 +20,7 @@
     <author>0171702</author>
   </authors>
   <commentList>
-    <comment ref="M30" authorId="0" shapeId="0">
+    <comment ref="M30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q94" authorId="0" shapeId="0">
+    <comment ref="Q94" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q97" authorId="0" shapeId="0">
+    <comment ref="Q97" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1806,7 +1801,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2040,7 +2035,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2082,7 +2077,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2117,7 +2112,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2328,11 +2323,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="H36" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="23.125" style="6" customWidth="1"/>
     <col min="2" max="2" width="12" style="6" customWidth="1"/>
@@ -2666,7 +2661,7 @@
     <col min="16135" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -2698,15 +2693,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" s="6" customFormat="1"/>
+    <row r="3" spans="1:25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="1"/>
       <c r="Y3" s="1"/>
     </row>
-    <row r="4" spans="1:25" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" s="8" customFormat="1" ht="12">
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10" t="s">
@@ -2734,7 +2729,7 @@
       <c r="W4" s="10"/>
       <c r="X4" s="12"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2780,7 +2775,7 @@
         <v xml:space="preserve">rails generate scaffold Company name:string category:string </v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" s="8" customFormat="1" ht="12">
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="10" t="s">
@@ -2812,7 +2807,7 @@
       <c r="W6" s="10"/>
       <c r="X6" s="12"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2866,7 +2861,7 @@
         <v xml:space="preserve">rails generate scaffold Location postcode:string address:string phoneNo:string destinationName:string </v>
       </c>
     </row>
-    <row r="8" spans="1:25" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" s="8" customFormat="1" ht="12">
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="10" t="s">
@@ -2892,7 +2887,7 @@
       <c r="W8" s="10"/>
       <c r="X8" s="12"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -2932,7 +2927,7 @@
         <v xml:space="preserve">rails generate scaffold Enginestatus name:string </v>
       </c>
     </row>
-    <row r="10" spans="1:25" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" s="8" customFormat="1" ht="12">
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10" t="s">
@@ -2958,7 +2953,7 @@
       <c r="W10" s="10"/>
       <c r="X10" s="12"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2998,7 +2993,7 @@
         <v xml:space="preserve">rails generate scaffold Businessstatus name:string </v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" s="8" customFormat="1" ht="12">
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
@@ -3026,7 +3021,7 @@
       <c r="W12" s="10"/>
       <c r="X12" s="12"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25">
       <c r="A13" s="1" t="s">
         <v>111</v>
       </c>
@@ -3070,7 +3065,7 @@
         <v xml:space="preserve">rails generate scaffold Engine engineModelName:string salesModelName:string </v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" s="8" customFormat="1" ht="12">
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="10" t="s">
@@ -3098,7 +3093,7 @@
       <c r="W14" s="10"/>
       <c r="X14" s="12"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -3142,19 +3137,19 @@
         <v xml:space="preserve">rails generate scaffold Enginemodel modelcode:string name:string </v>
       </c>
     </row>
-    <row r="16" spans="1:25" s="13" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" s="13" customFormat="1" ht="12">
       <c r="F16" s="14"/>
       <c r="H16" s="14"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:39">
       <c r="A17" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:39" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:39" s="8" customFormat="1" ht="12">
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10" t="s">
@@ -3184,7 +3179,7 @@
       <c r="W18" s="10"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:39">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -3232,7 +3227,7 @@
         <v xml:space="preserve">rails generate scaffold Returning returnDate:date returningComment:text sendingComment:text </v>
       </c>
     </row>
-    <row r="20" spans="1:39" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:39" s="8" customFormat="1" ht="12">
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
         <v>0</v>
@@ -3262,7 +3257,7 @@
       <c r="W20" s="10"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:39">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -3308,7 +3303,7 @@
         <v xml:space="preserve">rails generate scaffold Arrival arrivalDate:date arrivalComment:text </v>
       </c>
     </row>
-    <row r="22" spans="1:39" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:39" s="8" customFormat="1" ht="12">
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="20" t="s">
@@ -3346,7 +3341,7 @@
       <c r="W22" s="10"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:39">
       <c r="A23" s="1" t="s">
         <v>39</v>
       </c>
@@ -3410,7 +3405,7 @@
         <v xml:space="preserve">rails generate scaffold Repair issueNo:string issueDate:date arriveDate:date startDate:date finishDate:date beforeComment:text afterComment:text </v>
       </c>
     </row>
-    <row r="24" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:39" s="8" customFormat="1">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="10" t="s">
@@ -3464,7 +3459,7 @@
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:39">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
@@ -3544,7 +3539,7 @@
       <c r="AL25" s="8"/>
       <c r="AM25" s="8"/>
     </row>
-    <row r="26" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:39" s="8" customFormat="1">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="3"/>
@@ -3582,7 +3577,7 @@
       <c r="AL26" s="1"/>
       <c r="AM26" s="1"/>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:39">
       <c r="A27" s="1" t="s">
         <v>74</v>
       </c>
@@ -3611,7 +3606,7 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="8"/>
     </row>
-    <row r="28" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:39" s="8" customFormat="1">
       <c r="C28" s="9"/>
       <c r="D28" s="9" t="s">
         <v>0</v>
@@ -3641,7 +3636,7 @@
         <v xml:space="preserve">rails generate scaffold  </v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:39">
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
@@ -3674,7 +3669,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="8"/>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:39">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
@@ -3721,7 +3716,7 @@
       <c r="X30" s="5"/>
       <c r="Y30" s="1"/>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:39">
       <c r="A31" s="1" t="s">
         <v>163</v>
       </c>
@@ -3791,7 +3786,7 @@
         <v xml:space="preserve">rails generate scaffold Inquiry loginUserId:integer branchCode:integer userId:integer placeCode:integer orderer:string machineNo:string timeOfRunning:integer dayOfTest:date changeComment:text </v>
       </c>
     </row>
-    <row r="32" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:39" s="8" customFormat="1">
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="3"/>
@@ -3816,7 +3811,7 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="1"/>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4"/>
@@ -3846,7 +3841,7 @@
         <v xml:space="preserve">rails generate scaffold  </v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:25" s="8" customFormat="1">
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
@@ -3871,7 +3866,7 @@
       <c r="X34" s="12"/>
       <c r="Y34" s="1"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4"/>
@@ -3901,7 +3896,7 @@
         <v xml:space="preserve">rails generate scaffold  </v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4"/>
@@ -3931,13 +3926,13 @@
         <v xml:space="preserve">rails generate scaffold  </v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:25">
       <c r="D37" s="6" t="s">
         <v>0</v>
       </c>
       <c r="Y37" s="8"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:25">
       <c r="A38" s="7" t="s">
         <v>77</v>
       </c>
@@ -3949,14 +3944,14 @@
         <v xml:space="preserve">rails generate scaffold  </v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="15" thickBot="1">
       <c r="B39" s="6" t="s">
         <v>78</v>
       </c>
       <c r="C39" s="1"/>
       <c r="Y39" s="13"/>
     </row>
-    <row r="40" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="15" thickBot="1">
       <c r="C40" s="16" t="s">
         <v>79</v>
       </c>
@@ -3965,7 +3960,7 @@
         <v xml:space="preserve">rails generate scaffold rails generate devise:install </v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="18" thickBot="1">
       <c r="C41" s="16" t="s">
         <v>80</v>
       </c>
@@ -3974,7 +3969,7 @@
       </c>
       <c r="Y41" s="13"/>
     </row>
-    <row r="42" spans="1:25" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25" ht="17.25">
       <c r="C42" s="6" t="s">
         <v>81</v>
       </c>
@@ -3986,7 +3981,7 @@
         <v>rails generate scaffold rails g devise:views # =&gt; すべてテーブルの内容が tmp/fixtures/*.yml に抽出される</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25" ht="17.25">
       <c r="C43" s="6" t="s">
         <v>82</v>
       </c>
@@ -3994,12 +3989,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:25" ht="17.25">
       <c r="K44" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="15" thickBot="1">
       <c r="B45" s="6" t="s">
         <v>83</v>
       </c>
@@ -4007,12 +4002,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="15" thickBot="1">
       <c r="C46" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="15" thickBot="1">
       <c r="C47" s="17" t="s">
         <v>86</v>
       </c>
@@ -4020,17 +4015,17 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="15" thickBot="1">
       <c r="C48" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12">
       <c r="K49" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" ht="17.25">
       <c r="B50" s="6" t="s">
         <v>87</v>
       </c>
@@ -4038,12 +4033,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:12">
       <c r="C51" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:12">
       <c r="C52" s="6" t="s">
         <v>89</v>
       </c>
@@ -4054,7 +4049,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:12" ht="17.25">
       <c r="C53" s="6" t="s">
         <v>90</v>
       </c>
@@ -4062,107 +4057,107 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:12">
       <c r="A55" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="15" thickBot="1">
       <c r="B56" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="15" thickBot="1">
       <c r="C57" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="15" thickBot="1">
       <c r="B58" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="15" thickBot="1">
       <c r="C59" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="15" thickBot="1">
       <c r="B60" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="15" thickBot="1">
       <c r="C61" s="17" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="15" thickBot="1">
       <c r="B62" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="15" thickBot="1">
       <c r="C63" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="15" thickBot="1">
       <c r="B64" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C64" s="19"/>
     </row>
-    <row r="65" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" ht="15" thickBot="1">
       <c r="C65" s="17" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:25">
       <c r="C66" s="19"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:25">
       <c r="C67" s="19"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:25">
       <c r="C68" s="19"/>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:25">
       <c r="A69" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" ht="15" thickBot="1">
       <c r="B70" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" ht="15" thickBot="1">
       <c r="C71" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" ht="15" thickBot="1">
       <c r="B73" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" ht="15" thickBot="1">
       <c r="C74" s="17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:25">
       <c r="B76" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:25">
       <c r="C77" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:25">
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="20" t="s">
@@ -4207,7 +4202,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:25">
       <c r="C80" s="4" t="s">
         <v>35</v>
       </c>
@@ -4269,12 +4264,12 @@
         <v xml:space="preserve">rails g migration add_attrs1_to_repairs  timeOfRunning:integer dayOfTest:date arrivalComment:text orderNo:string orderDate:date constructionNo:string desirableFinishDate:date estimatedFinishDate:date </v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:26">
       <c r="B82" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:26">
       <c r="E83" s="6" t="s">
         <v>159</v>
       </c>
@@ -4282,7 +4277,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:26">
       <c r="C84" s="4" t="s">
         <v>35</v>
       </c>
@@ -4298,12 +4293,12 @@
         <v xml:space="preserve"> returningComment:text </v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:26">
       <c r="B87" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:26" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:26" s="8" customFormat="1" ht="12">
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="10" t="s">
@@ -4335,7 +4330,7 @@
       <c r="W88" s="10"/>
       <c r="X88" s="12"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:26">
       <c r="A89" s="1"/>
       <c r="B89" s="15"/>
       <c r="C89" s="4" t="s">
@@ -4385,20 +4380,20 @@
         <v xml:space="preserve">rails g migration add_locationcols_to_companies postcode:string address:string phoneNo:string destinationName:string </v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:26">
       <c r="Y90" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:26">
       <c r="Y91"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:26">
       <c r="B92" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:26">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="4"/>
@@ -4448,7 +4443,7 @@
       <c r="Y94" s="3"/>
       <c r="Z94" s="5"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:26">
       <c r="A95" s="1" t="s">
         <v>163</v>
       </c>
@@ -4522,7 +4517,7 @@
       <c r="Y95" s="3"/>
       <c r="Z95" s="5"/>
     </row>
-    <row r="97" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="97" spans="2:26">
       <c r="E97" s="3" t="s">
         <v>197</v>
       </c>
@@ -4556,7 +4551,7 @@
       <c r="Y97" s="3"/>
       <c r="Z97" s="5"/>
     </row>
-    <row r="98" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="98" spans="2:26">
       <c r="E98" s="10" t="s">
         <v>198</v>
       </c>
@@ -4600,41 +4595,41 @@
       <c r="Y98" s="3"/>
       <c r="Z98" s="5"/>
     </row>
-    <row r="100" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="100" spans="2:26">
       <c r="E100" s="6" t="str">
         <f>CONCATENATE($A$1,C95," ",E95,F95,G95,H95,I95,J95,K95,L95,M95,N95,O95,P95,Q95,R95,S95,T95,U95,V95,W95,X95,Y95,Z95) &amp; CONCATENATE(E98,F98,G98,H98,I98,J98,K98,L98)</f>
         <v xml:space="preserve">rails generate scaffold Engineorder issueNo:string inquiryDate:date loginUserId:integer branchCode:integer userId:integer placeCode:integer orderer:string machineNo:string timeOfRunning:integer changeComment:text orderDate:date sendingCompanyCode:integer sendingComment:text deliveryDate:date </v>
       </c>
     </row>
-    <row r="102" spans="2:26" x14ac:dyDescent="0.15">
+    <row r="102" spans="2:26">
       <c r="C102" s="24" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:26" ht="15" thickBot="1">
       <c r="B103" s="6" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="104" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:26" ht="15" thickBot="1">
       <c r="C104" s="17" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:26" ht="15" thickBot="1">
       <c r="C105" s="17" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="106" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:26" ht="15" thickBot="1">
       <c r="C106" s="17"/>
     </row>
-    <row r="107" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:26" ht="15" thickBot="1">
       <c r="B107" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:26" ht="15" thickBot="1">
       <c r="C108" s="17" t="s">
         <v>207</v>
       </c>
@@ -4642,7 +4637,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="109" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:26" ht="15" thickBot="1">
       <c r="C109" s="17" t="s">
         <v>208</v>
       </c>
@@ -4651,33 +4646,33 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="111" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="112" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:26" ht="15" thickBot="1"/>
+    <row r="112" spans="2:26" ht="15" thickBot="1">
       <c r="C112" s="17" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:27" ht="15" thickBot="1">
       <c r="C113" s="17" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="115" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="115" spans="2:27">
       <c r="B115" s="6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="116" spans="2:27">
       <c r="C116" s="6" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="118" spans="2:27">
       <c r="B118" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="119" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="119" spans="2:27">
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
       <c r="E119" s="10" t="s">
@@ -4712,7 +4707,7 @@
       <c r="Z119" s="8"/>
       <c r="AA119" s="8"/>
     </row>
-    <row r="120" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="120" spans="2:27">
       <c r="C120" s="4" t="s">
         <v>199</v>
       </c>
@@ -4760,7 +4755,7 @@
         <v xml:space="preserve">rails g migration add_locationcols_to_companies returning_date:string returning_comment:textinvoice_no_new:string invoice_no_old:string </v>
       </c>
     </row>
-    <row r="121" spans="2:27" x14ac:dyDescent="0.15">
+    <row r="121" spans="2:27">
       <c r="Y121" s="6" t="s">
         <v>162</v>
       </c>
@@ -4782,9 +4777,9 @@
       <selection activeCell="C1" sqref="C1:W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="9"/>
@@ -4829,7 +4824,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="14.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" ht="14.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -4895,7 +4890,7 @@
         <v xml:space="preserve">rails g migration add_attrs1_to_repairs  timeOfRunning:integer dayOfTest:date arrivalComment:text orderNo:string orderDate:date constructionNo:string desirableFinishDate:date estimatedFinishDate:date </v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23">
       <c r="E3" t="s">
         <v>129</v>
       </c>
@@ -4918,52 +4913,52 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23">
       <c r="I4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23">
       <c r="I5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23">
       <c r="I6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23">
       <c r="I7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23">
       <c r="I8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23">
       <c r="I9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23">
       <c r="I10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23">
       <c r="I11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23">
       <c r="I12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23">
       <c r="I15" t="s">
         <v>130</v>
       </c>

</xml_diff>